<commit_message>
Update of main readme and template files
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -60,9 +60,6 @@
     <t>period</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
     <t>doi</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>euro</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,31 +441,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed templates to sek
</commit_message>
<xml_diff>
--- a/template/template.xlsx
+++ b/template/template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28008"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulfkro/OneDrive/KB-dokument/Open Access/Kostnader/Open APC Sweden/openapc-se/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camlin\system\openapc-se\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38060" windowHeight="23260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38055" windowHeight="23265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,10 @@
   <definedNames>
     <definedName name="template" localSheetId="0">Blad1!$A$1:$K$2</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,13 +84,13 @@
     <t>url</t>
   </si>
   <si>
-    <t>euro</t>
+    <t>sek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -140,6 +140,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -418,22 +421,22 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>